<commit_message>
update data after run
</commit_message>
<xml_diff>
--- a/data/All_MDA_Data.xlsx
+++ b/data/All_MDA_Data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -685,13 +685,13 @@
         <v>79.59999999999999</v>
       </c>
       <c r="AB2" t="n">
-        <v>65.13286639616399</v>
+        <v>64.37435589208292</v>
       </c>
       <c r="AC2" t="n">
-        <v>3.166056375924171</v>
+        <v>3.949086466552615</v>
       </c>
       <c r="AD2" t="n">
-        <v>14.36719601620658</v>
+        <v>13.45632043806779</v>
       </c>
       <c r="AE2" t="n">
         <v>75.04895106481463</v>
@@ -700,116 +700,10 @@
         <v>4.174360848444937</v>
       </c>
       <c r="AG2" t="n">
-        <v>81.43328102219211</v>
+        <v>81.428519079832</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.572607569240667</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>UK026</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>69.381059496383</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2.990408785214228</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.5444530740673791</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G3" t="n">
-        <v>81.2617215227487</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1.362491930577165</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1.002336842002403</v>
-      </c>
-      <c r="J3" t="n">
-        <v>44</v>
-      </c>
-      <c r="K3" t="n">
-        <v>95.03524191820603</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1.392330498191732</v>
-      </c>
-      <c r="M3" t="n">
-        <v>5.759330453162659</v>
-      </c>
-      <c r="N3" t="n">
-        <v>147</v>
-      </c>
-      <c r="O3" t="n">
-        <v>69.381059496383</v>
-      </c>
-      <c r="P3" t="n">
-        <v>2.990408785214228</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.5444530740673791</v>
-      </c>
-      <c r="R3" t="n">
-        <v>3</v>
-      </c>
-      <c r="S3" t="n">
-        <v>80.82319989141254</v>
-      </c>
-      <c r="T3" t="n">
-        <v>1.375466356075473</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0.9520498527593673</v>
-      </c>
-      <c r="V3" t="n">
-        <v>43</v>
-      </c>
-      <c r="W3" t="n">
-        <v>72.60084917609576</v>
-      </c>
-      <c r="X3" t="n">
-        <v>2.230118492877943</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>0.717506213458649</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>6</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>89.59999999999999</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>65.21266578989312</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>4.510256927765283</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>9.111540937138514</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>66.88788283496321</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>4.613232793338047</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>87.0272363590194</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>1.00740493017476</v>
+        <v>0.572542084751227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>